<commit_message>
Updated Evap slides 8 and 16 + spreadsheet
Calc basis for changes off of Historical
Look at wintertime precipt and evap
</commit_message>
<xml_diff>
--- a/3 - Post Processing/WillardBayEvapScratch/WillardBayEvaporation.xlsx
+++ b/3 - Post Processing/WillardBayEvapScratch/WillardBayEvaporation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\WeberBasinWCD\WeberDroughtVulnerability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\WeberBasinWCD\WeberDroughtVulnerability\JacobCode\GitHub\3 - Post Processing\WillardBayEvapScratch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D6EE0C-50B2-4C83-8F4C-BAB75A45388F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B91EA84-1029-4C35-AD17-910AAE626C9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>month</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Volume @ Full (ac-feet)</t>
   </si>
   <si>
-    <t>Change in vol [ac-feet]</t>
-  </si>
-  <si>
     <t>Incremental volum (ac-feet)</t>
   </si>
   <si>
@@ -234,6 +231,24 @@
   </si>
   <si>
     <t>$/ac-ft</t>
+  </si>
+  <si>
+    <t>Percent change from</t>
+  </si>
+  <si>
+    <t>Historical</t>
+  </si>
+  <si>
+    <t>Change in volume from [ac-feet]</t>
+  </si>
+  <si>
+    <t>NET EVAP (No winter precip or evap)</t>
+  </si>
+  <si>
+    <t>All values in feet</t>
+  </si>
+  <si>
+    <t>Winter (Months 11, 12, 1, 2)</t>
   </si>
 </sst>
 </file>
@@ -907,7 +922,6 @@
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -988,6 +1002,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2662,29 +2679,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" style="4"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+    <col min="17" max="17" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -2697,9 +2714,9 @@
       <c r="M3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="12"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q3" s="11"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2733,11 +2750,11 @@
       <c r="N4" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2771,11 +2788,11 @@
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2809,11 +2826,11 @@
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2847,11 +2864,11 @@
       <c r="N7">
         <v>0.02</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2885,11 +2902,11 @@
       <c r="N8">
         <v>0.15</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2923,11 +2940,11 @@
       <c r="N9">
         <v>0.33</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="Q9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2961,9 +2978,9 @@
       <c r="N10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2997,11 +3014,11 @@
       <c r="N11">
         <v>0.81</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="Q11" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3035,9 +3052,9 @@
       <c r="N12">
         <v>0.7</v>
       </c>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3071,11 +3088,11 @@
       <c r="N13">
         <v>0.41</v>
       </c>
-      <c r="Q13" s="8" t="s">
+      <c r="Q13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3109,9 +3126,9 @@
       <c r="N14">
         <v>0.18</v>
       </c>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3145,11 +3162,11 @@
       <c r="N15">
         <v>0</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="Q15" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3183,631 +3200,734 @@
       <c r="N16">
         <v>0</v>
       </c>
-      <c r="Q16" s="9"/>
-    </row>
-    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="Q17" s="10" t="s">
+      <c r="Q16" s="8"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q17" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q18" s="11"/>
-    </row>
-    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="Q19" s="10" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q18" s="10"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40" t="s">
+      <c r="D20" s="39"/>
+      <c r="E20" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40" t="s">
+      <c r="F20" s="39"/>
+      <c r="G20" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="40"/>
-      <c r="Q20" s="10" t="s">
+      <c r="H20" s="39"/>
+      <c r="Q20" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="18" t="s">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" s="39"/>
+      <c r="B21" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Q21" s="7"/>
-    </row>
-    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="Q21" s="6"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" s="12">
         <f t="shared" ref="A22:A33" si="0">A5</f>
         <v>1</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <f t="shared" ref="B22:B33" si="1">N5</f>
         <v>0</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <f t="shared" ref="C22:D33" si="2">CONVERT(B5/1000,"m","ft")</f>
         <v>0.28215223097112857</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <f t="shared" si="2"/>
         <v>7.5459317585301833E-2</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="13">
         <f t="shared" ref="E22:F33" si="3">CONVERT(F5/1000,"m","ft")</f>
         <v>0.31496062992125984</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="13">
         <f t="shared" si="3"/>
         <v>7.874015748031496E-2</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <f t="shared" ref="G22:G33" si="4">CONVERT(J5/1000,"m","ft")</f>
         <v>0.30183727034120733</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="13">
         <f t="shared" ref="H22:H33" si="5">CONVERT(K5/1000,"m","ft")</f>
         <v>8.2020997375328086E-2</v>
       </c>
-      <c r="Q22" s="8" t="s">
+      <c r="Q22" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <f t="shared" si="2"/>
         <v>0.19685039370078741</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="13">
         <f t="shared" si="2"/>
         <v>9.8425196850393706E-2</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="13">
         <f t="shared" si="3"/>
         <v>0.23950131233595801</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="13">
         <f t="shared" si="3"/>
         <v>0.10498687664041995</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <f t="shared" si="4"/>
         <v>0.21653543307086615</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H23" s="13">
         <f t="shared" si="5"/>
         <v>0.11482939632545934</v>
       </c>
-      <c r="Q23" s="7"/>
-    </row>
-    <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="Q23" s="6"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="13">
         <f t="shared" si="2"/>
         <v>0.15091863517060367</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="13">
         <f t="shared" si="2"/>
         <v>0.20013123359580051</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <f t="shared" si="3"/>
         <v>0.14107611548556429</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="13">
         <f t="shared" si="3"/>
         <v>0.20997375328083989</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <f t="shared" si="4"/>
         <v>0.12795275590551181</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="13">
         <f t="shared" si="5"/>
         <v>0.24934383202099739</v>
       </c>
-      <c r="Q24" s="8" t="s">
+      <c r="Q24" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="12">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="13">
         <f t="shared" si="2"/>
         <v>0.13451443569553806</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="13">
         <f t="shared" si="2"/>
         <v>0.3543307086614173</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="13">
         <f t="shared" si="3"/>
         <v>0.14107611548556429</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="13">
         <f t="shared" si="3"/>
         <v>0.36745406824146981</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <f t="shared" si="4"/>
         <v>0.13451443569553806</v>
       </c>
-      <c r="H25" s="14">
+      <c r="H25" s="13">
         <f t="shared" si="5"/>
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="13">
         <f t="shared" si="2"/>
         <v>0.12467191601049869</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="13">
         <f t="shared" si="2"/>
         <v>0.49540682414698162</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="13">
         <f t="shared" si="3"/>
         <v>0.11811023622047244</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="13">
         <f t="shared" si="3"/>
         <v>0.52165354330708658</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <f t="shared" si="4"/>
         <v>0.11811023622047244</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="13">
         <f t="shared" si="5"/>
         <v>0.57742782152230976</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="12">
         <f t="shared" si="1"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="13">
         <f t="shared" si="2"/>
         <v>5.57742782152231E-2</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="13">
         <f t="shared" si="2"/>
         <v>0.74146981627296593</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="13">
         <f t="shared" si="3"/>
         <v>3.937007874015748E-2</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="13">
         <f t="shared" si="3"/>
         <v>0.76443569553805779</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <f t="shared" si="4"/>
         <v>4.2650918635170607E-2</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="13">
         <f t="shared" si="5"/>
         <v>0.81692913385826771</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="12">
         <f t="shared" si="1"/>
         <v>0.81</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="13">
         <f t="shared" si="2"/>
         <v>9.8425196850393699E-3</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="13">
         <f t="shared" si="2"/>
         <v>0.83005249343832022</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="13">
         <f t="shared" si="3"/>
         <v>1.968503937007874E-2</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="13">
         <f t="shared" si="3"/>
         <v>0.84317585301837272</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <f t="shared" si="4"/>
         <v>1.6404199475065617E-2</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="13">
         <f t="shared" si="5"/>
         <v>0.8923884514435696</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="12">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="13">
         <f t="shared" si="2"/>
         <v>1.3123359580052493E-2</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="13">
         <f t="shared" si="2"/>
         <v>0.88910761154855644</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="13">
         <f t="shared" si="3"/>
         <v>1.3123359580052493E-2</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="13">
         <f t="shared" si="3"/>
         <v>0.90551181102362199</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <f t="shared" si="4"/>
         <v>1.6404199475065617E-2</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="13">
         <f t="shared" si="5"/>
         <v>0.90551181102362199</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <f t="shared" si="1"/>
         <v>0.41</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="13">
         <f t="shared" si="2"/>
         <v>5.2493438320209973E-2</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <f t="shared" si="2"/>
         <v>0.6889763779527559</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="13">
         <f t="shared" si="3"/>
         <v>5.905511811023622E-2</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="13">
         <f t="shared" si="3"/>
         <v>0.70866141732283461</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <f t="shared" si="4"/>
         <v>9.514435695538058E-2</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="13">
         <f t="shared" si="5"/>
         <v>0.67913385826771655</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="12">
         <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="13">
         <f t="shared" si="2"/>
         <v>7.217847769028872E-2</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="13">
         <f t="shared" si="2"/>
         <v>0.45931758530183736</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="13">
         <f t="shared" si="3"/>
         <v>7.5459317585301833E-2</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="13">
         <f t="shared" si="3"/>
         <v>0.47244094488188976</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <f t="shared" si="4"/>
         <v>7.5459317585301833E-2</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="13">
         <f t="shared" si="5"/>
         <v>0.44291338582677164</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="13">
         <f t="shared" si="2"/>
         <v>0.11482939632545934</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="13">
         <f t="shared" si="2"/>
         <v>0.23293963254593172</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="13">
         <f t="shared" si="3"/>
         <v>0.11482939632545934</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="13">
         <f t="shared" si="3"/>
         <v>0.24278215223097113</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <f t="shared" si="4"/>
         <v>0.14107611548556429</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="13">
         <f t="shared" si="5"/>
         <v>0.2230971128608924</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="13">
         <f t="shared" si="2"/>
         <v>0.26246719160104987</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="13">
         <f t="shared" si="2"/>
         <v>0.13123359580052493</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="13">
         <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="13">
         <f t="shared" si="3"/>
         <v>0.13123359580052493</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <f t="shared" si="4"/>
         <v>0.29199475065616798</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="13">
         <f t="shared" si="5"/>
         <v>0.13451443569553806</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="15">
         <f>SUM(B22:B33)</f>
         <v>3.1500000000000004</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="15">
         <f t="shared" ref="C34:H34" si="6">SUM(C22:C33)</f>
         <v>1.4698162729658795</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="15">
         <f t="shared" si="6"/>
         <v>5.1968503937007879</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="15">
         <f t="shared" si="6"/>
         <v>1.5387139107611549</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="15">
         <f t="shared" si="6"/>
         <v>5.3510498687664043</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="15">
         <f t="shared" si="6"/>
         <v>1.5780839895013123</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="15">
         <f t="shared" si="6"/>
         <v>5.5347769028871383</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="15">
         <f>B34</f>
         <v>3.1500000000000004</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="16">
+      <c r="C35" s="14"/>
+      <c r="D35" s="15">
         <f>D34-C34</f>
         <v>3.7270341207349085</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16">
+      <c r="E35" s="14"/>
+      <c r="F35" s="15">
         <f>F34-E34</f>
         <v>3.8123359580052494</v>
       </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="16">
+      <c r="G35" s="14"/>
+      <c r="H35" s="15">
         <f>H34-G34</f>
         <v>3.956692913385826</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="40">
+        <f>SUM(B22:B23,B32:B33)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="40">
+        <f t="shared" ref="C36:H36" si="7">SUM(C22:C23,C32:C33)</f>
+        <v>0.85629921259842523</v>
+      </c>
+      <c r="D36" s="40">
+        <f t="shared" si="7"/>
+        <v>0.53805774278215224</v>
+      </c>
+      <c r="E36" s="40">
+        <f t="shared" si="7"/>
+        <v>0.93175853018372701</v>
+      </c>
+      <c r="F36" s="40">
+        <f t="shared" si="7"/>
+        <v>0.55774278215223094</v>
+      </c>
+      <c r="G36" s="40">
+        <f t="shared" si="7"/>
+        <v>0.95144356955380582</v>
+      </c>
+      <c r="H36" s="40">
+        <f t="shared" si="7"/>
+        <v>0.5544619422572179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="40">
+        <f>B35</f>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="D37" s="40">
+        <f>D35+C36-D36</f>
+        <v>4.0452755905511815</v>
+      </c>
+      <c r="F37" s="40">
+        <f>F35+E36-F36</f>
+        <v>4.1863517060367448</v>
+      </c>
+      <c r="H37" s="40">
+        <f>H35+G36-H36</f>
+        <v>4.3536745406824142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="H38" s="40"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D40" s="18">
         <f>(H35-D35)/D35</f>
         <v>6.1619718309858844E-2</v>
       </c>
-      <c r="H38" s="19"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="36">
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="35">
         <f>(D35-$B$35)/$B$35</f>
         <v>0.18318543515393906</v>
       </c>
-      <c r="F39" s="36">
+      <c r="F42" s="35">
         <f>(F35-$B$35)/$B$35</f>
         <v>0.21026538349372983</v>
       </c>
-      <c r="H39" s="36">
+      <c r="H42" s="35">
         <f>(H35-$B$35)/$B$35</f>
         <v>0.25609298837645256</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="35"/>
+      <c r="F43" s="35">
+        <f>(F35-$D$35)/$D$35</f>
+        <v>2.2887323943661889E-2</v>
+      </c>
+      <c r="H43" s="35">
+        <f>(H35-$D$35)/$D$35</f>
+        <v>6.1619718309858844E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="37">
+      <c r="B45" s="36">
         <f>B35*WillardBayVolumes!$I$35</f>
         <v>31405.499999978143</v>
       </c>
-      <c r="D41" s="37">
+      <c r="D45" s="36">
         <f>D35*WillardBayVolumes!$I$35</f>
         <v>37158.530183701172</v>
       </c>
-      <c r="F41" s="37">
+      <c r="F45" s="36">
         <f>F35*WillardBayVolumes!$I$35</f>
         <v>38008.989501285883</v>
       </c>
-      <c r="H41" s="37">
+      <c r="H45" s="36">
         <f>H35*WillardBayVolumes!$I$35</f>
         <v>39448.228346429227</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="38">
-        <f>D41-$B$41</f>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="H46" s="36"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="37">
+        <f>D45-$B$45</f>
         <v>5753.030183723029</v>
       </c>
-      <c r="F42" s="38">
-        <f>F41-$B$41</f>
+      <c r="F48" s="37">
+        <f>F$45-$B$45</f>
         <v>6603.4895013077403</v>
       </c>
-      <c r="H42" s="38">
-        <f>H41-$B$41</f>
+      <c r="H48" s="37">
+        <f>H45-$B$45</f>
         <v>8042.7283464510838</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="37"/>
+      <c r="F49" s="37">
+        <f>F$45-$D$45</f>
+        <v>850.45931758471124</v>
+      </c>
+      <c r="H49" s="37">
+        <f>H$45-$D$45</f>
+        <v>2289.6981627280547</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51">
         <v>300</v>
       </c>
-      <c r="D44" s="37">
-        <f>$B$44*D42</f>
+      <c r="D51" s="36">
+        <f>$B$51*D48</f>
         <v>1725909.0551169086</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37">
-        <f>$B$44*F42</f>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36">
+        <f>$B$51*F48</f>
         <v>1981046.8503923221</v>
       </c>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37">
-        <f>$B$44*H42</f>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36">
+        <f>$B$51*H48</f>
         <v>2412818.503935325</v>
       </c>
     </row>
@@ -3831,21 +3951,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E117AC3-1310-43F6-A710-EC7BEACFCE39}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -3853,57 +3973,57 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>32</v>
       </c>
       <c r="H3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>28</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>60</v>
       </c>
       <c r="H4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="26">
         <v>51</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <v>166</v>
       </c>
       <c r="H5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>96</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>495</v>
       </c>
       <c r="H6" t="s">
@@ -3913,20 +4033,20 @@
         <v>50</v>
       </c>
       <c r="J6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" t="s">
         <v>60</v>
       </c>
-      <c r="K6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="26">
         <v>160</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="27">
         <v>649</v>
       </c>
       <c r="H7">
@@ -3936,14 +4056,14 @@
         <v>261.00000000088897</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>255</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>820</v>
       </c>
       <c r="H8">
@@ -3952,23 +4072,23 @@
       <c r="I8">
         <v>1059.99999999901</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="38">
         <f>AVERAGE(I7:I8,)*(H8-H7)</f>
         <v>440.33333333329966</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="36">
         <f>SUM(J$8:J8)</f>
         <v>440.33333333329966</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>248</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <v>759</v>
       </c>
       <c r="H9">
@@ -3977,23 +4097,23 @@
       <c r="I9">
         <v>2209.999999999</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="38">
         <f t="shared" ref="J9:J35" si="0">AVERAGE(I8:I9,)*(H9-H8)</f>
         <v>1089.9999999993368</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="36">
         <f>SUM(J$8:J9)</f>
         <v>1530.3333333326364</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>139</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>621</v>
       </c>
       <c r="H10">
@@ -4002,23 +4122,23 @@
       <c r="I10">
         <v>4200.0000000049304</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="38">
         <f t="shared" si="0"/>
         <v>2136.6666666679771</v>
       </c>
-      <c r="K10" s="37">
+      <c r="K10" s="36">
         <f>SUM(J$8:J10)</f>
         <v>3667.0000000006135</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="26">
         <v>178</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="27">
         <v>161</v>
       </c>
       <c r="H11">
@@ -4027,23 +4147,23 @@
       <c r="I11">
         <v>6080.00000000196</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="38">
         <f t="shared" si="0"/>
         <v>3426.6666666689634</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="36">
         <f>SUM(J$8:J11)</f>
         <v>7093.6666666695764</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>198</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="24">
         <v>-112</v>
       </c>
       <c r="H12">
@@ -4052,23 +4172,23 @@
       <c r="I12">
         <v>6540.0000000009704</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="38">
         <f t="shared" si="0"/>
         <v>4206.6666666676438</v>
       </c>
-      <c r="K12" s="37">
+      <c r="K12" s="36">
         <f>SUM(J$8:J12)</f>
         <v>11300.333333337221</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="26">
         <v>118</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="27">
         <v>-190</v>
       </c>
       <c r="H13">
@@ -4077,23 +4197,23 @@
       <c r="I13">
         <v>7999.99999999998</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="38">
         <f t="shared" si="0"/>
         <v>4846.6666666669835</v>
       </c>
-      <c r="K13" s="37">
+      <c r="K13" s="36">
         <f>SUM(J$8:J13)</f>
         <v>16147.000000004206</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>86</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="24">
         <v>-92</v>
       </c>
       <c r="H14">
@@ -4102,23 +4222,23 @@
       <c r="I14">
         <v>8490.0000000059099</v>
       </c>
-      <c r="J14" s="39">
+      <c r="J14" s="38">
         <f t="shared" si="0"/>
         <v>5496.6666666686297</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K14" s="36">
         <f>SUM(J$8:J14)</f>
         <v>21643.666666672834</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="26">
         <v>8</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="27">
         <v>23</v>
       </c>
       <c r="H15">
@@ -4127,23 +4247,23 @@
       <c r="I15">
         <v>8830.0000000019609</v>
       </c>
-      <c r="J15" s="39">
+      <c r="J15" s="38">
         <f t="shared" si="0"/>
         <v>5773.3333333359578</v>
       </c>
-      <c r="K15" s="37">
+      <c r="K15" s="36">
         <f>SUM(J$8:J15)</f>
         <v>27417.000000008793</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="29">
         <v>1565</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="30">
         <v>3368</v>
       </c>
       <c r="H16">
@@ -4152,16 +4272,16 @@
       <c r="I16">
         <v>9080.0000000019609</v>
       </c>
-      <c r="J16" s="39">
+      <c r="J16" s="38">
         <f t="shared" si="0"/>
         <v>5970.0000000013069</v>
       </c>
-      <c r="K16" s="37">
+      <c r="K16" s="36">
         <f>SUM(J$8:J16)</f>
         <v>33387.000000010099</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17">
         <f>SUM(B4:B15)</f>
         <v>1565</v>
@@ -4176,32 +4296,32 @@
       <c r="I17">
         <v>9269.9999999881202</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="38">
         <f t="shared" si="0"/>
         <v>6116.666666663361</v>
       </c>
-      <c r="K17" s="37">
+      <c r="K17" s="36">
         <f>SUM(J$8:J17)</f>
         <v>39503.66666667346</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H18">
         <v>4210.99999999999</v>
       </c>
       <c r="I18">
         <v>9389.9999999910906</v>
       </c>
-      <c r="J18" s="39">
+      <c r="J18" s="38">
         <f t="shared" si="0"/>
         <v>6219.9999999930706</v>
       </c>
-      <c r="K18" s="37">
+      <c r="K18" s="36">
         <f>SUM(J$8:J18)</f>
         <v>45723.666666666533</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -4211,69 +4331,69 @@
       <c r="I19">
         <v>9490.0000000059099</v>
       </c>
-      <c r="J19" s="39">
+      <c r="J19" s="38">
         <f t="shared" si="0"/>
         <v>6293.3333333323344</v>
       </c>
-      <c r="K19" s="37">
+      <c r="K19" s="36">
         <f>SUM(J$8:J19)</f>
         <v>52016.999999998865</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H20">
         <v>4212.99999999999</v>
       </c>
       <c r="I20">
         <v>9580.0000000019609</v>
       </c>
-      <c r="J20" s="39">
+      <c r="J20" s="38">
         <f t="shared" si="0"/>
         <v>6356.6666666692909</v>
       </c>
-      <c r="K20" s="37">
+      <c r="K20" s="36">
         <f>SUM(J$8:J20)</f>
         <v>58373.666666668156</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="H21" s="35">
+      <c r="D21" s="33"/>
+      <c r="H21" s="34">
         <v>4213.99999999999</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="34">
         <v>9660.0000000039308</v>
       </c>
-      <c r="J21" s="39">
+      <c r="J21" s="38">
         <f t="shared" si="0"/>
         <v>6413.3333333352975</v>
       </c>
-      <c r="K21" s="37">
+      <c r="K21" s="36">
         <f>SUM(J$8:J21)</f>
         <v>64787.000000003456</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="33">
+      <c r="B22" s="32">
         <v>4229</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <f>B$17/VLOOKUP(B22,$H$7:$I$35,2)</f>
         <v>0.15697091273832389</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <f>C$17/$I$35</f>
         <v>0.33701103309953245</v>
       </c>
@@ -4283,27 +4403,27 @@
       <c r="I22">
         <v>9719.9999999930606</v>
       </c>
-      <c r="J22" s="39">
+      <c r="J22" s="38">
         <f t="shared" si="0"/>
         <v>6459.9999999989968</v>
       </c>
-      <c r="K22" s="37">
+      <c r="K22" s="36">
         <f>SUM(J$8:J22)</f>
         <v>71247.000000002459</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="33">
+      <c r="B23" s="32">
         <v>4201</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <f>B$17/$I$8</f>
         <v>1.4764150943410015</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="13">
         <f>C$17/$I$8</f>
         <v>3.1698113207576775</v>
       </c>
@@ -4313,192 +4433,192 @@
       <c r="I23">
         <v>9759.9999999940501</v>
       </c>
-      <c r="J23" s="39">
+      <c r="J23" s="38">
         <f t="shared" si="0"/>
         <v>6493.3333333290366</v>
       </c>
-      <c r="K23" s="37">
+      <c r="K23" s="36">
         <f>SUM(J$8:J23)</f>
         <v>77740.333333331495</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H24">
         <v>4216.99999999999</v>
       </c>
       <c r="I24">
         <v>9790.0000000009695</v>
       </c>
-      <c r="J24" s="39">
+      <c r="J24" s="38">
         <f t="shared" si="0"/>
         <v>6516.6666666650062</v>
       </c>
-      <c r="K24" s="37">
+      <c r="K24" s="36">
         <f>SUM(J$8:J24)</f>
         <v>84256.999999996508</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H25">
         <v>4217.99999999999</v>
       </c>
       <c r="I25">
         <v>9809.9999999891097</v>
       </c>
-      <c r="J25" s="39">
+      <c r="J25" s="38">
         <f t="shared" si="0"/>
         <v>6533.3333333300261</v>
       </c>
-      <c r="K25" s="37">
+      <c r="K25" s="36">
         <f>SUM(J$8:J25)</f>
         <v>90790.333333326533</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H26">
         <v>4218.99999999999</v>
       </c>
       <c r="I26">
         <v>9839.9999999960291</v>
       </c>
-      <c r="J26" s="39">
+      <c r="J26" s="38">
         <f t="shared" si="0"/>
         <v>6549.999999995046</v>
       </c>
-      <c r="K26" s="37">
+      <c r="K26" s="36">
         <f>SUM(J$8:J26)</f>
         <v>97340.333333321585</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H27">
         <v>4219.99999999999</v>
       </c>
       <c r="I27">
         <v>9860.0000000088803</v>
       </c>
-      <c r="J27" s="39">
+      <c r="J27" s="38">
         <f t="shared" si="0"/>
         <v>6566.6666666683041</v>
       </c>
-      <c r="K27" s="37">
+      <c r="K27" s="36">
         <f>SUM(J$8:J27)</f>
         <v>103906.99999998989</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H28">
         <v>4220.99999999999</v>
       </c>
       <c r="I28">
         <v>9879.9999999970205</v>
       </c>
-      <c r="J28" s="39">
+      <c r="J28" s="38">
         <f t="shared" si="0"/>
         <v>6580.0000000019672</v>
       </c>
-      <c r="K28" s="37">
+      <c r="K28" s="36">
         <f>SUM(J$8:J28)</f>
         <v>110486.99999999185</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H29">
         <v>4221.99999999999</v>
       </c>
       <c r="I29">
         <v>9900.0000000098607</v>
       </c>
-      <c r="J29" s="39">
+      <c r="J29" s="38">
         <f t="shared" si="0"/>
         <v>6593.3333333356277</v>
       </c>
-      <c r="K29" s="37">
+      <c r="K29" s="36">
         <f>SUM(J$8:J29)</f>
         <v>117080.33333332748</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H30">
         <v>4222.99999999999</v>
       </c>
       <c r="I30">
         <v>9919.9999999979991</v>
       </c>
-      <c r="J30" s="39">
+      <c r="J30" s="38">
         <f t="shared" si="0"/>
         <v>6606.6666666692863</v>
       </c>
-      <c r="K30" s="37">
+      <c r="K30" s="36">
         <f>SUM(J$8:J30)</f>
         <v>123686.99999999677</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H31">
         <v>4223.99999999999</v>
       </c>
       <c r="I31">
         <v>9929.9999999920801</v>
       </c>
-      <c r="J31" s="39">
+      <c r="J31" s="38">
         <f t="shared" si="0"/>
         <v>6616.66666666336</v>
       </c>
-      <c r="K31" s="37">
+      <c r="K31" s="36">
         <f>SUM(J$8:J31)</f>
         <v>130303.66666666012</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H32">
         <v>4224.99999999999</v>
       </c>
       <c r="I32">
         <v>9940.0000000108503</v>
       </c>
-      <c r="J32" s="39">
+      <c r="J32" s="38">
         <f t="shared" si="0"/>
         <v>6623.3333333343107</v>
       </c>
-      <c r="K32" s="37">
+      <c r="K32" s="36">
         <f>SUM(J$8:J32)</f>
         <v>136926.99999999444</v>
       </c>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.35">
       <c r="H33">
         <v>4225.99999999999</v>
       </c>
       <c r="I33">
         <v>9950.0000000049204</v>
       </c>
-      <c r="J33" s="39">
+      <c r="J33" s="38">
         <f t="shared" si="0"/>
         <v>6630.0000000052569</v>
       </c>
-      <c r="K33" s="37">
+      <c r="K33" s="36">
         <f>SUM(J$8:J33)</f>
         <v>143556.99999999971</v>
       </c>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.35">
       <c r="H34">
         <v>4227.99999999999</v>
       </c>
       <c r="I34">
         <v>9969.9999999930606</v>
       </c>
-      <c r="J34" s="39">
+      <c r="J34" s="38">
         <f t="shared" si="0"/>
         <v>13279.999999998654</v>
       </c>
-      <c r="K34" s="37">
+      <c r="K34" s="36">
         <f>SUM(J$8:J34)</f>
         <v>156836.99999999837</v>
       </c>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D35">
         <v>33000</v>
       </c>
@@ -4508,16 +4628,16 @@
       <c r="I35">
         <v>9969.9999999930606</v>
       </c>
-      <c r="J35" s="39">
+      <c r="J35" s="38">
         <f t="shared" si="0"/>
         <v>6646.6666666620404</v>
       </c>
-      <c r="K35" s="37">
+      <c r="K35" s="36">
         <f>SUM(J$8:J35)</f>
         <v>163483.6666666604</v>
       </c>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D36">
         <f>D35/I35</f>
         <v>3.309929789370408</v>

</xml_diff>

<commit_message>
Workable shortage contour plots (in code file 4e)
Average annual shortage (column 1) and max shortage (in Column 2) Shortages reported in 1,000 acre-feet/year
</commit_message>
<xml_diff>
--- a/3 - Post Processing/WillardBayEvapScratch/WillardBayEvaporation.xlsx
+++ b/3 - Post Processing/WillardBayEvapScratch/WillardBayEvaporation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\WeberBasinWCD\WeberDroughtVulnerability\JacobCode\GitHub\3 - Post Processing\WillardBayEvapScratch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194CF822-CBAE-4CC6-BED2-F4594A6FA6DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DD8D0A-2480-41A7-8B17-1E716946C534}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>month</t>
   </si>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>Winter (Months 11, 12, 1, 2)</t>
+  </si>
+  <si>
+    <t>Wholesale water values (Jon, WBWCD, February 28, 2019) [$/acre-feet]</t>
+  </si>
+  <si>
+    <t>Low priority water</t>
+  </si>
+  <si>
+    <t>High priroity water</t>
   </si>
 </sst>
 </file>
@@ -2679,17 +2688,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.1796875" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="12.1796875" customWidth="1"/>
     <col min="8" max="8" width="11.54296875" customWidth="1"/>
@@ -3914,21 +3923,42 @@
         <v>61</v>
       </c>
       <c r="B51">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D51" s="36">
         <f>$B$51*D48</f>
-        <v>1725909.0551169086</v>
+        <v>2876515.0918615144</v>
       </c>
       <c r="E51" s="36"/>
       <c r="F51" s="36">
         <f>$B$51*F48</f>
-        <v>1981046.8503923221</v>
+        <v>3301744.7506538699</v>
       </c>
       <c r="G51" s="36"/>
       <c r="H51" s="36">
         <f>$B$51*H48</f>
-        <v>2412818.503935325</v>
+        <v>4021364.1732255421</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>500</v>
+      </c>
+      <c r="B57" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>